<commit_message>
matrix concept comparison script and outputs
</commit_message>
<xml_diff>
--- a/benchmarking_example/error_analysis_template.xlsx
+++ b/benchmarking_example/error_analysis_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11102"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rastegar-a/Documents/GitHub/i-adopt-llm-based-service/benchmarking_example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C49A967C-B1FF-EA4D-967E-8DDB947A3E3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B6C7F3A-7839-F742-A865-74FE631D72A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Error Analysis" sheetId="1" r:id="rId1"/>
@@ -1022,13 +1022,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="34.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="38.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" style="1"/>
+    <col min="4" max="4" width="25.83203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="99.5" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="32" x14ac:dyDescent="0.2">

</xml_diff>